<commit_message>
Demo is now complete
</commit_message>
<xml_diff>
--- a/demoData/toy cement/toycement_unitlibrary.xlsx
+++ b/demoData/toy cement/toycement_unitlibrary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/demoData/toy cement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAE23A1-7D00-864D-B5FA-90D809192EA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33596B66-F7FB-E84B-A8D1-C42FDE8D84E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="1560" windowWidth="27640" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Processes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -109,28 +109,40 @@
     <t>var meal mixer</t>
   </si>
   <si>
-    <t>units/cementUnits.xlsx</t>
-  </si>
-  <si>
-    <t>units/auxUnits.xlsx</t>
+    <t>c CO2 Compression</t>
+  </si>
+  <si>
+    <t>v CO2 Compression</t>
+  </si>
+  <si>
+    <t>c Power Station</t>
+  </si>
+  <si>
+    <t>v Power Station</t>
+  </si>
+  <si>
+    <t>mysterious_cement_factory</t>
+  </si>
+  <si>
+    <t>this factory is very mysterious</t>
+  </si>
+  <si>
+    <t>c mystery factory</t>
+  </si>
+  <si>
+    <t>var mystery factory</t>
+  </si>
+  <si>
+    <t>demoData/toy cement/units/cementUnits.xlsx</t>
+  </si>
+  <si>
+    <t>demoData/toy cement/units/auxUnits.xlsx</t>
+  </si>
+  <si>
+    <t>v CO2 Capture</t>
   </si>
   <si>
     <t>c CO2 Capture</t>
-  </si>
-  <si>
-    <t>v CO2 capture</t>
-  </si>
-  <si>
-    <t>c CO2 Compression</t>
-  </si>
-  <si>
-    <t>v CO2 Compression</t>
-  </si>
-  <si>
-    <t>c Power Station</t>
-  </si>
-  <si>
-    <t>v Power Station</t>
   </si>
 </sst>
 </file>
@@ -972,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,13 +1029,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>23</v>
@@ -1043,13 +1055,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>24</v>
@@ -1069,13 +1081,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>25</v>
@@ -1095,16 +1107,16 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>9</v>
@@ -1121,16 +1133,16 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
@@ -1147,19 +1159,45 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>